<commit_message>
wrote down all data
</commit_message>
<xml_diff>
--- a/Assignment1/utilities/data/analysis.xlsx
+++ b/Assignment1/utilities/data/analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14140" yWindow="0" windowWidth="14620" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="11860" yWindow="0" windowWidth="16900" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="11">
   <si>
     <t>Train %</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>Neighbours</t>
+  </si>
+  <si>
+    <t>Kernel</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>Polynomial</t>
   </si>
 </sst>
 </file>
@@ -91,8 +100,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -132,7 +155,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -149,6 +172,13 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -165,6 +195,13 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -494,16 +531,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="K94" sqref="K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
     <col min="8" max="8" width="13.83203125" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1810,7 +1849,7 @@
         <v>0.99942870745060697</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:11">
       <c r="B65">
         <v>2</v>
       </c>
@@ -1830,7 +1869,7 @@
         <v>0.99936749753459997</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:11">
       <c r="B66">
         <v>3</v>
       </c>
@@ -1850,7 +1889,7 @@
         <v>0.99941510524705002</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:11">
       <c r="B67">
         <v>4</v>
       </c>
@@ -1870,7 +1909,7 @@
         <v>0.99931988982215103</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:11">
       <c r="A68">
         <v>60</v>
       </c>
@@ -1896,7 +1935,7 @@
         <v>0.99951031900676302</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:11">
       <c r="B69">
         <v>2</v>
       </c>
@@ -1916,7 +1955,7 @@
         <v>0.99938789875845402</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:11">
       <c r="B70">
         <v>3</v>
       </c>
@@ -1936,7 +1975,7 @@
         <v>0.99946951225732705</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:11">
       <c r="B71">
         <v>4</v>
       </c>
@@ -1956,7 +1995,7 @@
         <v>0.99933689032165895</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:11">
       <c r="A72">
         <v>80</v>
       </c>
@@ -1982,7 +2021,7 @@
         <v>0.99951032400228501</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:11">
       <c r="B73">
         <v>2</v>
       </c>
@@ -2002,7 +2041,7 @@
         <v>0.99955113033542797</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:11">
       <c r="B74">
         <v>3</v>
       </c>
@@ -2022,7 +2061,7 @@
         <v>0.99959193666857005</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:11">
       <c r="B75">
         <v>4</v>
       </c>
@@ -2042,8 +2081,450 @@
         <v>0.99944911450257001</v>
       </c>
     </row>
+    <row r="77" spans="1:11">
+      <c r="A77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="G77" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" t="s">
+        <v>2</v>
+      </c>
+      <c r="E78" t="s">
+        <v>3</v>
+      </c>
+      <c r="G78" t="s">
+        <v>0</v>
+      </c>
+      <c r="H78" t="s">
+        <v>6</v>
+      </c>
+      <c r="I78" t="s">
+        <v>8</v>
+      </c>
+      <c r="J78" t="s">
+        <v>2</v>
+      </c>
+      <c r="K78" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79">
+        <v>20</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79">
+        <v>0.52351190476190401</v>
+      </c>
+      <c r="E79">
+        <v>0.53313253012048101</v>
+      </c>
+      <c r="G79">
+        <v>20</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79" t="s">
+        <v>9</v>
+      </c>
+      <c r="J79">
+        <v>0.45938989825114901</v>
+      </c>
+      <c r="K79">
+        <v>0.49355763443273498</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="C80" t="s">
+        <v>10</v>
+      </c>
+      <c r="D80">
+        <v>0.52351190476190401</v>
+      </c>
+      <c r="E80">
+        <v>0.53313253012048101</v>
+      </c>
+      <c r="I80" t="s">
+        <v>10</v>
+      </c>
+      <c r="J80">
+        <v>0.445960964538549</v>
+      </c>
+      <c r="K80">
+        <v>0.55493098558501497</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="B81">
+        <v>100</v>
+      </c>
+      <c r="C81" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81">
+        <v>0.753571428571428</v>
+      </c>
+      <c r="E81">
+        <v>0.81777108433734902</v>
+      </c>
+      <c r="H81">
+        <v>100</v>
+      </c>
+      <c r="I81" t="s">
+        <v>9</v>
+      </c>
+      <c r="J81">
+        <v>0.81822506417044605</v>
+      </c>
+      <c r="K81">
+        <v>0.84184324087203999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="C82" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82">
+        <v>0.48005952380952299</v>
+      </c>
+      <c r="E82">
+        <v>0.73343373493975905</v>
+      </c>
+      <c r="I82" t="s">
+        <v>10</v>
+      </c>
+      <c r="J82">
+        <v>0.67067132570613197</v>
+      </c>
+      <c r="K82">
+        <v>0.18086571518929201</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
+      <c r="A83">
+        <v>40</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83">
+        <v>0.64759036144578297</v>
+      </c>
+      <c r="E83">
+        <v>0.63855421686746905</v>
+      </c>
+      <c r="G83">
+        <v>40</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83" t="s">
+        <v>9</v>
+      </c>
+      <c r="J83">
+        <v>0.43002235102617598</v>
+      </c>
+      <c r="K83">
+        <v>0.48693848403441298</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
+      <c r="C84" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84">
+        <v>0.60843373493975905</v>
+      </c>
+      <c r="E84">
+        <v>0.60441767068273</v>
+      </c>
+      <c r="I84" t="s">
+        <v>10</v>
+      </c>
+      <c r="J84">
+        <v>0.38307852739176002</v>
+      </c>
+      <c r="K84">
+        <v>0.359764681878464</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="B85">
+        <v>100</v>
+      </c>
+      <c r="C85" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85">
+        <v>0.79819277108433695</v>
+      </c>
+      <c r="E85">
+        <v>0.59036144578313199</v>
+      </c>
+      <c r="H85">
+        <v>100</v>
+      </c>
+      <c r="I85" t="s">
+        <v>9</v>
+      </c>
+      <c r="J85">
+        <v>0.52866364384728004</v>
+      </c>
+      <c r="K85">
+        <v>0.50434930458734295</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
+      <c r="C86" t="s">
+        <v>10</v>
+      </c>
+      <c r="D86">
+        <v>0.69277108433734902</v>
+      </c>
+      <c r="E86">
+        <v>0.74297188755020005</v>
+      </c>
+      <c r="I86" t="s">
+        <v>10</v>
+      </c>
+      <c r="J86">
+        <v>0.53029288299314803</v>
+      </c>
+      <c r="K86">
+        <v>0.89931648927126195</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
+      <c r="A87">
+        <v>60</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87" t="s">
+        <v>9</v>
+      </c>
+      <c r="D87">
+        <v>0.531983739837398</v>
+      </c>
+      <c r="E87">
+        <v>0.469879518072289</v>
+      </c>
+      <c r="G87">
+        <v>60</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87" t="s">
+        <v>9</v>
+      </c>
+      <c r="J87">
+        <v>0.74262640619903697</v>
+      </c>
+      <c r="K87">
+        <v>0.81096273323607704</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
+      <c r="C88" t="s">
+        <v>10</v>
+      </c>
+      <c r="D88">
+        <v>0.531983739837398</v>
+      </c>
+      <c r="E88">
+        <v>0.469879518072289</v>
+      </c>
+      <c r="I88" t="s">
+        <v>10</v>
+      </c>
+      <c r="J88">
+        <v>0.72516533305119901</v>
+      </c>
+      <c r="K88">
+        <v>0.68763453475204706</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
+      <c r="B89">
+        <v>100</v>
+      </c>
+      <c r="C89" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89">
+        <v>0.63195121951219502</v>
+      </c>
+      <c r="E89">
+        <v>0.43975903614457801</v>
+      </c>
+      <c r="H89">
+        <v>100</v>
+      </c>
+      <c r="I89" t="s">
+        <v>9</v>
+      </c>
+      <c r="J89">
+        <v>0.33872362199169798</v>
+      </c>
+      <c r="K89">
+        <v>0.60560276669761104</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="C90" t="s">
+        <v>10</v>
+      </c>
+      <c r="D90">
+        <v>0.66473170731707298</v>
+      </c>
+      <c r="E90">
+        <v>0.73795180722891496</v>
+      </c>
+      <c r="I90" t="s">
+        <v>10</v>
+      </c>
+      <c r="J90">
+        <v>0.531902780699408</v>
+      </c>
+      <c r="K90">
+        <v>0.77025800067331096</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
+      <c r="A91">
+        <v>80</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91">
+        <v>0.577309018326982</v>
+      </c>
+      <c r="E91">
+        <v>0.48795180722891501</v>
+      </c>
+      <c r="G91">
+        <v>80</v>
+      </c>
+      <c r="H91">
+        <v>1</v>
+      </c>
+      <c r="I91" t="s">
+        <v>9</v>
+      </c>
+      <c r="J91">
+        <v>0.43272628746974701</v>
+      </c>
+      <c r="K91">
+        <v>0.67995592916020497</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
+      <c r="C92" t="s">
+        <v>10</v>
+      </c>
+      <c r="D92">
+        <v>0.621928869533659</v>
+      </c>
+      <c r="E92">
+        <v>0.71084337349397497</v>
+      </c>
+      <c r="I92" t="s">
+        <v>10</v>
+      </c>
+      <c r="J92">
+        <v>0.67497454219164299</v>
+      </c>
+      <c r="K92">
+        <v>0.57428792948665597</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="B93">
+        <v>100</v>
+      </c>
+      <c r="C93" t="s">
+        <v>9</v>
+      </c>
+      <c r="D93">
+        <v>0.75307566684812199</v>
+      </c>
+      <c r="E93">
+        <v>0.40361445783132499</v>
+      </c>
+      <c r="H93">
+        <v>100</v>
+      </c>
+      <c r="I93" t="s">
+        <v>9</v>
+      </c>
+      <c r="J93">
+        <v>0.67688925843791703</v>
+      </c>
+      <c r="K93">
+        <v>0.53448135150575304</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="C94" t="s">
+        <v>10</v>
+      </c>
+      <c r="D94">
+        <v>0.64184358555615995</v>
+      </c>
+      <c r="E94">
+        <v>0.52409638554216798</v>
+      </c>
+      <c r="I94" t="s">
+        <v>10</v>
+      </c>
+      <c r="J94">
+        <v>0.59867321063393297</v>
+      </c>
+      <c r="K94">
+        <v>0.87423488125356996</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A77:E77"/>
+    <mergeCell ref="G77:K77"/>
     <mergeCell ref="A58:D58"/>
     <mergeCell ref="F58:I58"/>
     <mergeCell ref="A1:D1"/>

</xml_diff>